<commit_message>
split reading of excel files in a nodes sheet and edge sheet
</commit_message>
<xml_diff>
--- a/data/network-structure-1.xlsx
+++ b/data/network-structure-1.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bramvanmeurs/stack/EPA/Afstuderen - EPA/code/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B8B05C-F6F1-304A-BDC6-E6E75472D8BD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF118B8F-8AEA-FF43-98B6-53B2D1FB12A9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="300" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="edges" sheetId="1" r:id="rId1"/>
-    <sheet name="nodes" sheetId="2" r:id="rId2"/>
+    <sheet name="nodes" sheetId="2" r:id="rId1"/>
+    <sheet name="edges" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -30,9 +30,6 @@
   </si>
   <si>
     <t>pnode</t>
-  </si>
-  <si>
-    <t>type</t>
   </si>
   <si>
     <t>A.1</t>
@@ -932,336 +929,461 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F98BEFE-4D84-7B41-AB14-29EC8A040C97}">
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="6" max="8" width="11" customWidth="1"/>
+    <col min="4" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
         <v>19</v>
       </c>
       <c r="F1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>0.2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>0.2</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>0.2</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>0.2</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>0.2</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>0.2</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>0.2</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>0.2</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="E2">
-        <v>7</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <v>20</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10">
         <v>0.2</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7">
-        <v>0.2</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8">
-        <v>0.2</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-      <c r="J8">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9">
-        <v>0.2</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>3</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10">
-        <v>0.2</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>2</v>
-      </c>
-      <c r="J10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11">
-        <v>0.2</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12">
-        <v>0.2</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13">
-        <v>0.2</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>4</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14">
-        <v>0.2</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>5</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
+      <c r="F10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F98BEFE-4D84-7B41-AB14-29EC8A040C97}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added bifurcation option to main script, also rewritten the calculation order to take into account multiple sinks
</commit_message>
<xml_diff>
--- a/data/network-structure-1.xlsx
+++ b/data/network-structure-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bramvanmeurs/stack/EPA/Afstuderen - EPA/code/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF118B8F-8AEA-FF43-98B6-53B2D1FB12A9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7534717D-4125-E248-AF58-2DE1211B8B22}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="300" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="2" r:id="rId1"/>
@@ -932,7 +932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F98BEFE-4D84-7B41-AB14-29EC8A040C97}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -1200,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1239,6 +1239,9 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
       <c r="E2">
         <v>0.2</v>
       </c>
@@ -1256,6 +1259,9 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
       <c r="E3">
         <v>0.2</v>
       </c>
@@ -1273,6 +1279,9 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
       <c r="E4">
         <v>0.2</v>
       </c>
@@ -1290,6 +1299,9 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
       <c r="E5">
         <v>0.2</v>
       </c>
@@ -1307,6 +1319,9 @@
       <c r="C6" t="s">
         <v>14</v>
       </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
       <c r="E6">
         <v>0.2</v>
       </c>
@@ -1324,6 +1339,9 @@
       <c r="C7" t="s">
         <v>14</v>
       </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
       <c r="E7">
         <v>0.2</v>
       </c>
@@ -1341,6 +1359,9 @@
       <c r="C8" t="s">
         <v>5</v>
       </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
       <c r="E8">
         <v>0.2</v>
       </c>
@@ -1358,6 +1379,9 @@
       <c r="C9" t="s">
         <v>6</v>
       </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
       <c r="E9">
         <v>0.2</v>
       </c>
@@ -1374,6 +1398,9 @@
       </c>
       <c r="C10" t="s">
         <v>15</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
       </c>
       <c r="E10">
         <v>0.2</v>

</xml_diff>